<commit_message>
Added .gitkeep file, Changed .properties to .ini, Added assertion condition, Added another testcase
</commit_message>
<xml_diff>
--- a/Test_Data_For_Automating_Sales_Module.xlsx
+++ b/Test_Data_For_Automating_Sales_Module.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t xml:space="preserve">                Test Cases and Results</t>
   </si>
@@ -96,10 +96,16 @@
     <t>7. Enter Down Payment</t>
   </si>
   <si>
-    <t>It should create the order</t>
-  </si>
-  <si>
     <t>Ram Laptop Distributor</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC_Sales_001_2</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -260,6 +266,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,11 +281,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1 2" xfId="1"/>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -576,40 +582,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="14"/>
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -647,109 +653,199 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>44557</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" s="9" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" s="9" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1">
         <v>11</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7">
+        <v>44557</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1">
+        <v>11</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="E7:E13"/>
@@ -760,6 +856,11 @@
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="G14:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added new testcase, Removed print statement, Changed some conditions
</commit_message>
<xml_diff>
--- a/Test_Data_For_Automating_Sales_Module.xlsx
+++ b/Test_Data_For_Automating_Sales_Module.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t xml:space="preserve">                Test Cases and Results</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_Sales_001_3</t>
+  </si>
+  <si>
+    <t>Azure</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -844,23 +850,125 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="7">
+        <v>44558</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1">
+        <v>12</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="20">
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="G14:G20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:G3"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="E7:E13"/>
     <mergeCell ref="F7:F13"/>
     <mergeCell ref="G7:G13"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="G14:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>